<commit_message>
Updated some of the sheets
</commit_message>
<xml_diff>
--- a/streaming/iex_fx_quotes.xlsx
+++ b/streaming/iex_fx_quotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\xlslim-code-samples\streaming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A7142A-1B15-4E58-AACD-148CEF6B37C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCABF1C5-6952-4DA3-8F41-695A36AE352C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6831" yWindow="3283" windowWidth="24686" windowHeight="13054" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
+    <workbookView xWindow="3429" yWindow="2006" windowWidth="24685" windowHeight="13054" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -251,6 +251,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -263,7 +264,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
@@ -288,12 +288,12 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv_a0d343074d8a4242bb7340eebf21676e">
+    <main first="rtdsrv_c644d2bedd18402e9a115c4bc7fe82c5">
       <tp t="s">
-        <v>iex_fx_quote/"GBPUSD"@517</v>
+        <v>RTD/1634059158@111</v>
         <stp/>
         <stp>iex_fx_quote</stp>
-        <stp>"GBPUSD"</stp>
+        <stp>1634059158</stp>
         <tr r="B7" s="1"/>
       </tp>
     </main>
@@ -601,7 +601,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -620,16 +620,16 @@
         <f t="array" ref="B1">_xll.WorkbookLocation()</f>
         <v>D:\github\xlslim-code-samples\streaming</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
@@ -639,14 +639,14 @@
         <f>B1&amp;"\iex_fx_quotes.py"</f>
         <v>D:\github\xlslim-code-samples\streaming\iex_fx_quotes.py</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -656,34 +656,34 @@
         <f t="array" ref="B3">_xll.RegisterPyModule(B2)</f>
         <v>Registered D:\github\xlslim-code-samples\streaming\iex_fx_quotes.py</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:12" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
@@ -692,17 +692,17 @@
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
@@ -713,19 +713,19 @@
         <v>GBPUSD</v>
       </c>
       <c r="C7" s="2" t="str">
-        <v>2022-07-27 13:37:20</v>
+        <v>2022-07-29 12:04:23</v>
       </c>
       <c r="D7" s="2">
-        <v>1.21123</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="9"/>
+        <v>1.23167</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -737,18 +737,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -884,14 +884,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -903,6 +895,14 @@
     <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Bloomberg sample is done
</commit_message>
<xml_diff>
--- a/streaming/iex_fx_quotes.xlsx
+++ b/streaming/iex_fx_quotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\xlslim-code-samples\streaming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCABF1C5-6952-4DA3-8F41-695A36AE352C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4830E50-1FE8-45D5-B68A-606EA0D7397F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3429" yWindow="2006" windowWidth="24685" windowHeight="13054" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
+    <workbookView xWindow="4277" yWindow="2503" windowWidth="24686" windowHeight="13054" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -288,9 +288,9 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv_c644d2bedd18402e9a115c4bc7fe82c5">
+    <main first="rtdsrv_67c7a2cd584e47fea7a77895f65ff862">
       <tp t="s">
-        <v>RTD/1634059158@111</v>
+        <v>RTD/1634059158@167</v>
         <stp/>
         <stp>iex_fx_quote</stp>
         <stp>1634059158</stp>
@@ -601,7 +601,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -713,10 +713,10 @@
         <v>GBPUSD</v>
       </c>
       <c r="C7" s="2" t="str">
-        <v>2022-07-29 12:04:23</v>
+        <v>2022-08-10 09:50:15</v>
       </c>
       <c r="D7" s="2">
-        <v>1.23167</v>
+        <v>1.2133499999999999</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -743,15 +743,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056A28DAB99C48B469009752D21F8474A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3725108ba1e248dd961cbde49d36f75">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="58a034177a2e5a667d336d2ca3036430" ns3:_="">
     <xsd:import namespace="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
@@ -883,6 +874,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
   <ds:schemaRefs>
@@ -900,14 +900,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C9D94B-68A3-4C5A-8543-29DBB1AA8066}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -923,4 +915,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update IEX examples to show they no longer work as the IEX sandbox environment is deprecated.
</commit_message>
<xml_diff>
--- a/streaming/iex_fx_quotes.xlsx
+++ b/streaming/iex_fx_quotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\xlslim-code-samples\streaming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4830E50-1FE8-45D5-B68A-606EA0D7397F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C664622-4D3A-471E-BCDA-15099F0EFE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4277" yWindow="2503" windowWidth="24686" windowHeight="13054" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Workbook location</t>
   </si>
@@ -85,12 +85,15 @@
   <si>
     <t>GBPUSD</t>
   </si>
+  <si>
+    <t>2023-03-22 - This code is no longer working, it looks like IEX do not offer their sandbox environment anymore.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,8 +140,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +182,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -235,14 +258,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -264,9 +288,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
+    <cellStyle name="Bad" xfId="5" builtinId="27"/>
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Input" xfId="4" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -283,22 +311,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
-<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <volType type="realTimeData">
-    <main first="rtdsrv_67c7a2cd584e47fea7a77895f65ff862">
-      <tp t="s">
-        <v>RTD/1634059158@167</v>
-        <stp/>
-        <stp>iex_fx_quote</stp>
-        <stp>1634059158</stp>
-        <tr r="B7" s="1"/>
-      </tp>
-    </main>
-  </volType>
-</volTypes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774E7E1C-D275-4DD4-9028-FA14541EA3B8}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -612,49 +624,42 @@
     <col min="4" max="4" width="27.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" ht="34.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="str" cm="1">
-        <f t="array" ref="B1">_xll.WorkbookLocation()</f>
-        <v>D:\github\xlslim-code-samples\streaming</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="B2" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="B2" ca="1">_xll.WorkbookLocation()</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="8"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="str">
-        <f>B1&amp;"\iex_fx_quotes.py"</f>
-        <v>D:\github\xlslim-code-samples\streaming\iex_fx_quotes.py</v>
-      </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="str" cm="1">
-        <f t="array" ref="B3">_xll.RegisterPyModule(B2)</f>
-        <v>Registered D:\github\xlslim-code-samples\streaming\iex_fx_quotes.py</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="e">
+        <f ca="1">B2&amp;"\iex_fx_quotes.py"</f>
+        <v>#NAME?</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -666,6 +671,13 @@
       <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="B4" ca="1">_xll.RegisterPyModule(B3)</f>
+        <v>#NAME?</v>
+      </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -675,7 +687,7 @@
       <c r="K4" s="9"/>
       <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="1:12" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -685,16 +697,7 @@
       <c r="K5" s="9"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>6</v>
-      </c>
+    <row r="6" spans="1:12" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -706,17 +709,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="str" cm="1">
-        <f t="array" ref="B7:D7">_xll.display_fx_quote(_xll.iex_fx_quote(B6))</f>
-        <v>GBPUSD</v>
-      </c>
-      <c r="C7" s="2" t="str">
-        <v>2022-08-10 09:50:15</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.2133499999999999</v>
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -727,9 +726,29 @@
       <c r="K7" s="9"/>
       <c r="L7" s="10"/>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="B8" ca="1">_xll.display_fx_quote(_xll.iex_fx_quote(B7))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E1:L7"/>
+  <mergeCells count="2">
+    <mergeCell ref="E2:L8"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -737,12 +756,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056A28DAB99C48B469009752D21F8474A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3725108ba1e248dd961cbde49d36f75">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="58a034177a2e5a667d336d2ca3036430" ns3:_="">
     <xsd:import namespace="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
@@ -874,6 +887,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -884,22 +903,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C9D94B-68A3-4C5A-8543-29DBB1AA8066}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -917,6 +920,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
   <ds:schemaRefs>

</xml_diff>